<commit_message>
Fixed Email field name in examples
</commit_message>
<xml_diff>
--- a/Employee/Example-EmployeeManagement-Employee-data.xlsx
+++ b/Employee/Example-EmployeeManagement-Employee-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\SAIGlobal\Compliance360-Import\Employee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18A05811-6F6B-4772-B44C-F92A119CCB25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36A1BF1-BE66-4627-B949-FB8E6700D969}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example-EmployeeManagement-Empl" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>Fax</t>
   </si>
   <si>
-    <t>Email Message</t>
-  </si>
-  <si>
     <t>Hire Date</t>
   </si>
   <si>
@@ -107,12 +104,15 @@
   </si>
   <si>
     <t>first.examplelast100003@mycompany.com</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -947,7 +947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -980,48 +980,48 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
       </c>
       <c r="J2" s="1">
         <v>40180</v>
@@ -1033,36 +1033,36 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
         <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
       </c>
       <c r="J3" s="1">
         <v>40180</v>
@@ -1074,36 +1074,36 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
         <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
       </c>
       <c r="J4" s="1">
         <v>40180</v>
@@ -1115,7 +1115,7 @@
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>